<commit_message>
WM8731 I2S 32bit frame working too, maybe required for input
</commit_message>
<xml_diff>
--- a/stm32f4-discovery-pin-table.xlsx
+++ b/stm32f4-discovery-pin-table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="256">
   <si>
     <t xml:space="preserve">Main function</t>
   </si>
@@ -899,7 +899,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">WM8731_SOUT?</t>
+    <t xml:space="preserve">WM8731_SOUT</t>
   </si>
   <si>
     <t xml:space="preserve">PB15</t>
@@ -940,7 +940,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">WM8731_SD (SIN?)</t>
+    <t xml:space="preserve">WM8731_SD (SIN)</t>
   </si>
   <si>
     <t xml:space="preserve">PC0</t>
@@ -1092,6 +1092,9 @@
 TIM3_CH3
 USART6_CK
 DCMI_D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_D0</t>
   </si>
   <si>
     <t xml:space="preserve">PC9</t>
@@ -1106,6 +1109,9 @@
 TIM3_CH4</t>
   </si>
   <si>
+    <t xml:space="preserve">SDIO_D1</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC10</t>
   </si>
   <si>
@@ -1145,6 +1151,9 @@
   </si>
   <si>
     <t xml:space="preserve">SCLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_D2</t>
   </si>
   <si>
     <t xml:space="preserve">PC11</t>
@@ -1158,6 +1167,9 @@
 I2S3ext_SD</t>
   </si>
   <si>
+    <t xml:space="preserve">SDIO_D3</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC12</t>
   </si>
   <si>
@@ -1199,6 +1211,9 @@
     <t xml:space="preserve">SDIN</t>
   </si>
   <si>
+    <t xml:space="preserve">SDIO_CK</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC13</t>
   </si>
   <si>
@@ -1244,6 +1259,9 @@
 UART5_RX
 SDIO_CMD
 DCMI_D11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_CMD</t>
   </si>
   <si>
     <t xml:space="preserve">PD3</t>
@@ -1864,9 +1882,9 @@
   <dimension ref="A1:S103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2990,7 +3008,7 @@
       </c>
       <c r="S33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="92.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
         <v>118</v>
       </c>
@@ -3023,7 +3041,7 @@
       </c>
       <c r="S34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
         <v>121</v>
       </c>
@@ -3057,7 +3075,7 @@
       <c r="S35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B36" s="17" t="s">
@@ -3313,7 +3331,7 @@
       </c>
       <c r="R43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="66.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="s">
         <v>145</v>
       </c>
@@ -3341,14 +3359,16 @@
       <c r="Q44" s="15" t="n">
         <v>45</v>
       </c>
-      <c r="R44" s="15"/>
-    </row>
-    <row r="45" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R44" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="92.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C45" s="15" t="n">
         <v>66</v>
@@ -3362,7 +3382,7 @@
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
       <c r="L45" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
@@ -3371,20 +3391,22 @@
       <c r="Q45" s="15" t="n">
         <v>46</v>
       </c>
-      <c r="R45" s="15"/>
-    </row>
-    <row r="46" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R45" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C46" s="7" t="n">
         <v>78</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="9"/>
@@ -3394,7 +3416,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
@@ -3403,14 +3425,16 @@
       <c r="Q46" s="7" t="n">
         <v>37</v>
       </c>
-      <c r="R46" s="7"/>
-    </row>
-    <row r="47" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R46" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="15" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C47" s="15" t="n">
         <v>79</v>
@@ -3424,7 +3448,7 @@
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
@@ -3433,20 +3457,22 @@
       <c r="Q47" s="15" t="n">
         <v>38</v>
       </c>
-      <c r="R47" s="15"/>
-    </row>
-    <row r="48" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R47" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C48" s="7" t="n">
         <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="9"/>
@@ -3456,7 +3482,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -3465,14 +3491,16 @@
       <c r="Q48" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="R48" s="7"/>
+      <c r="R48" s="10" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="15" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C49" s="15" t="n">
         <v>7</v>
@@ -3486,7 +3514,7 @@
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
       <c r="L49" s="15" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
@@ -3499,10 +3527,10 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="15" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C50" s="15" t="n">
         <v>8</v>
@@ -3515,10 +3543,10 @@
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="L50" s="15" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
@@ -3531,10 +3559,10 @@
     </row>
     <row r="51" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="15" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C51" s="15" t="n">
         <v>9</v>
@@ -3547,10 +3575,10 @@
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L51" s="15" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
@@ -3563,10 +3591,10 @@
     </row>
     <row r="52" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C52" s="15" t="n">
         <v>81</v>
@@ -3580,7 +3608,7 @@
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
       <c r="L52" s="15" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
@@ -3593,10 +3621,10 @@
     </row>
     <row r="53" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="15" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C53" s="15" t="n">
         <v>82</v>
@@ -3610,7 +3638,7 @@
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
       <c r="L53" s="15" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -3621,42 +3649,44 @@
       </c>
       <c r="R53" s="15"/>
     </row>
-    <row r="54" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C54" s="15" t="n">
+    <row r="54" customFormat="false" ht="53.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C54" s="10" t="n">
         <v>83</v>
       </c>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15" t="n">
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10" t="n">
         <v>34</v>
       </c>
-      <c r="R54" s="15"/>
+      <c r="R54" s="10" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C55" s="15" t="n">
         <v>84</v>
@@ -3670,7 +3700,7 @@
       <c r="J55" s="15"/>
       <c r="K55" s="15"/>
       <c r="L55" s="15" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
@@ -3683,10 +3713,10 @@
     </row>
     <row r="56" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C56" s="7" t="n">
         <v>85</v>
@@ -3702,7 +3732,7 @@
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
@@ -3715,10 +3745,10 @@
     </row>
     <row r="57" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C57" s="7" t="n">
         <v>86</v>
@@ -3728,15 +3758,15 @@
       <c r="F57" s="9"/>
       <c r="G57" s="7"/>
       <c r="H57" s="8" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I57" s="7"/>
       <c r="J57" s="8" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="K57" s="7"/>
       <c r="L57" s="7" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
@@ -3749,10 +3779,10 @@
     </row>
     <row r="58" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C58" s="15" t="n">
         <v>87</v>
@@ -3766,7 +3796,7 @@
       <c r="J58" s="15"/>
       <c r="K58" s="15"/>
       <c r="L58" s="15" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
@@ -3779,10 +3809,10 @@
     </row>
     <row r="59" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="15" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C59" s="15" t="n">
         <v>88</v>
@@ -3796,7 +3826,7 @@
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
@@ -3809,10 +3839,10 @@
     </row>
     <row r="60" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C60" s="10" t="n">
         <v>55</v>
@@ -3826,7 +3856,7 @@
       <c r="J60" s="10"/>
       <c r="K60" s="10"/>
       <c r="L60" s="10" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="M60" s="10"/>
       <c r="N60" s="10"/>
@@ -3836,15 +3866,15 @@
       </c>
       <c r="Q60" s="10"/>
       <c r="R60" s="10" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C61" s="10" t="n">
         <v>56</v>
@@ -3858,7 +3888,7 @@
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
       <c r="L61" s="10" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="M61" s="10"/>
       <c r="N61" s="10"/>
@@ -3868,15 +3898,15 @@
       </c>
       <c r="Q61" s="10"/>
       <c r="R61" s="10" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C62" s="15" t="n">
         <v>57</v>
@@ -3890,7 +3920,7 @@
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
       <c r="L62" s="15" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
@@ -3903,10 +3933,10 @@
     </row>
     <row r="63" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C63" s="15" t="n">
         <v>58</v>
@@ -3920,7 +3950,7 @@
       <c r="J63" s="15"/>
       <c r="K63" s="15"/>
       <c r="L63" s="15" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
@@ -3933,10 +3963,10 @@
     </row>
     <row r="64" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C64" s="10" t="n">
         <v>59</v>
@@ -3952,7 +3982,7 @@
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
       <c r="L64" s="10" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
@@ -3967,10 +3997,10 @@
     </row>
     <row r="65" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C65" s="10" t="n">
         <v>60</v>
@@ -3980,13 +4010,13 @@
       <c r="F65" s="11"/>
       <c r="G65" s="10"/>
       <c r="H65" s="12" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="I65" s="10"/>
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
       <c r="L65" s="10" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
@@ -4001,10 +4031,10 @@
     </row>
     <row r="66" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C66" s="10" t="n">
         <v>61</v>
@@ -4014,13 +4044,13 @@
       <c r="F66" s="11"/>
       <c r="G66" s="10"/>
       <c r="H66" s="12" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I66" s="10"/>
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
       <c r="L66" s="10" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
@@ -4035,10 +4065,10 @@
     </row>
     <row r="67" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C67" s="10" t="n">
         <v>62</v>
@@ -4048,13 +4078,13 @@
       <c r="F67" s="11"/>
       <c r="G67" s="10"/>
       <c r="H67" s="12" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="I67" s="10"/>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
       <c r="L67" s="10" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
@@ -4069,10 +4099,10 @@
     </row>
     <row r="68" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C68" s="15" t="n">
         <v>97</v>
@@ -4080,7 +4110,7 @@
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
       <c r="F68" s="16" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="15"/>
@@ -4088,7 +4118,7 @@
       <c r="J68" s="15"/>
       <c r="K68" s="15"/>
       <c r="L68" s="15" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
@@ -4101,10 +4131,10 @@
     </row>
     <row r="69" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C69" s="15" t="n">
         <v>98</v>
@@ -4112,7 +4142,7 @@
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
       <c r="F69" s="16" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="15"/>
@@ -4120,7 +4150,7 @@
       <c r="J69" s="15"/>
       <c r="K69" s="15"/>
       <c r="L69" s="15" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
@@ -4133,10 +4163,10 @@
     </row>
     <row r="70" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="15" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C70" s="15" t="n">
         <v>1</v>
@@ -4150,7 +4180,7 @@
       <c r="J70" s="15"/>
       <c r="K70" s="15"/>
       <c r="L70" s="15" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
@@ -4163,10 +4193,10 @@
     </row>
     <row r="71" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C71" s="15" t="n">
         <v>2</v>
@@ -4174,7 +4204,7 @@
       <c r="D71" s="15"/>
       <c r="E71" s="15"/>
       <c r="F71" s="16" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="15"/>
@@ -4182,7 +4212,7 @@
       <c r="J71" s="15"/>
       <c r="K71" s="15"/>
       <c r="L71" s="15" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
@@ -4195,10 +4225,10 @@
     </row>
     <row r="72" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="15" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C72" s="15" t="n">
         <v>3</v>
@@ -4212,7 +4242,7 @@
       <c r="J72" s="15"/>
       <c r="K72" s="15"/>
       <c r="L72" s="15" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
@@ -4225,10 +4255,10 @@
     </row>
     <row r="73" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C73" s="15" t="n">
         <v>4</v>
@@ -4242,7 +4272,7 @@
       <c r="J73" s="15"/>
       <c r="K73" s="15"/>
       <c r="L73" s="15" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
@@ -4255,10 +4285,10 @@
     </row>
     <row r="74" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="15" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="C74" s="15" t="n">
         <v>5</v>
@@ -4272,7 +4302,7 @@
       <c r="J74" s="15"/>
       <c r="K74" s="15"/>
       <c r="L74" s="15" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="M74" s="15"/>
       <c r="N74" s="15"/>
@@ -4285,10 +4315,10 @@
     </row>
     <row r="75" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="15" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C75" s="15" t="n">
         <v>38</v>
@@ -4302,7 +4332,7 @@
       <c r="J75" s="15"/>
       <c r="K75" s="15"/>
       <c r="L75" s="15" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
@@ -4315,10 +4345,10 @@
     </row>
     <row r="76" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="15" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C76" s="15" t="n">
         <v>39</v>
@@ -4332,7 +4362,7 @@
       <c r="J76" s="15"/>
       <c r="K76" s="15"/>
       <c r="L76" s="15" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
@@ -4345,10 +4375,10 @@
     </row>
     <row r="77" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="15" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C77" s="15" t="n">
         <v>40</v>
@@ -4362,7 +4392,7 @@
       <c r="J77" s="15"/>
       <c r="K77" s="15"/>
       <c r="L77" s="15" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
@@ -4375,10 +4405,10 @@
     </row>
     <row r="78" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="15" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C78" s="15" t="n">
         <v>41</v>
@@ -4392,7 +4422,7 @@
       <c r="J78" s="15"/>
       <c r="K78" s="15"/>
       <c r="L78" s="15" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
@@ -4405,10 +4435,10 @@
     </row>
     <row r="79" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="15" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C79" s="15" t="n">
         <v>42</v>
@@ -4422,7 +4452,7 @@
       <c r="J79" s="15"/>
       <c r="K79" s="15"/>
       <c r="L79" s="15" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
@@ -4435,10 +4465,10 @@
     </row>
     <row r="80" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="15" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C80" s="15" t="n">
         <v>43</v>
@@ -4452,7 +4482,7 @@
       <c r="J80" s="15"/>
       <c r="K80" s="15"/>
       <c r="L80" s="15" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="M80" s="15"/>
       <c r="N80" s="15"/>
@@ -4465,10 +4495,10 @@
     </row>
     <row r="81" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="15" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C81" s="15" t="n">
         <v>44</v>
@@ -4482,7 +4512,7 @@
       <c r="J81" s="15"/>
       <c r="K81" s="15"/>
       <c r="L81" s="15" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="M81" s="15"/>
       <c r="N81" s="15"/>
@@ -4495,10 +4525,10 @@
     </row>
     <row r="82" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="15" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C82" s="15" t="n">
         <v>45</v>
@@ -4512,7 +4542,7 @@
       <c r="J82" s="15"/>
       <c r="K82" s="15"/>
       <c r="L82" s="15" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="M82" s="15"/>
       <c r="N82" s="15"/>
@@ -4525,10 +4555,10 @@
     </row>
     <row r="83" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C83" s="15" t="n">
         <v>46</v>
@@ -4542,7 +4572,7 @@
       <c r="J83" s="15"/>
       <c r="K83" s="15"/>
       <c r="L83" s="15" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="M83" s="15"/>
       <c r="N83" s="15"/>
@@ -4555,10 +4585,10 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C84" s="7" t="n">
         <v>12</v>
@@ -4571,10 +4601,10 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="17" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="L84" s="7" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
@@ -4587,10 +4617,10 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C85" s="7" t="n">
         <v>13</v>
@@ -4603,10 +4633,10 @@
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
       <c r="K85" s="17" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L85" s="7" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
@@ -4631,7 +4661,7 @@
       <c r="K86" s="15"/>
       <c r="L86" s="15"/>
       <c r="M86" s="15" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N86" s="15"/>
       <c r="O86" s="15"/>
@@ -4655,7 +4685,7 @@
       <c r="K87" s="15"/>
       <c r="L87" s="15"/>
       <c r="M87" s="15" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N87" s="15"/>
       <c r="O87" s="15"/>
@@ -4679,7 +4709,7 @@
       <c r="K88" s="15"/>
       <c r="L88" s="15"/>
       <c r="M88" s="15" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="N88" s="15"/>
       <c r="O88" s="15"/>
@@ -4703,7 +4733,7 @@
       <c r="K89" s="15"/>
       <c r="L89" s="15"/>
       <c r="M89" s="15" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="N89" s="15"/>
       <c r="O89" s="15"/>
@@ -4727,7 +4757,7 @@
       <c r="K90" s="15"/>
       <c r="L90" s="15"/>
       <c r="M90" s="15" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="N90" s="15"/>
       <c r="O90" s="15"/>
@@ -4751,7 +4781,7 @@
       <c r="K91" s="15"/>
       <c r="L91" s="15"/>
       <c r="M91" s="15" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="N91" s="15"/>
       <c r="O91" s="15"/>
@@ -4775,7 +4805,7 @@
       <c r="K92" s="15"/>
       <c r="L92" s="15"/>
       <c r="M92" s="15" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="N92" s="15"/>
       <c r="O92" s="15"/>
@@ -4795,15 +4825,15 @@
       <c r="G93" s="15"/>
       <c r="H93" s="15"/>
       <c r="I93" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="J93" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="K93" s="15"/>
       <c r="L93" s="15"/>
       <c r="M93" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N93" s="15" t="n">
         <v>5</v>
@@ -4831,7 +4861,7 @@
       <c r="K94" s="15"/>
       <c r="L94" s="15"/>
       <c r="M94" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N94" s="15"/>
       <c r="O94" s="15"/>
@@ -4855,7 +4885,7 @@
       <c r="K95" s="15"/>
       <c r="L95" s="15"/>
       <c r="M95" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N95" s="15"/>
       <c r="O95" s="15"/>
@@ -4879,7 +4909,7 @@
       <c r="K96" s="15"/>
       <c r="L96" s="15"/>
       <c r="M96" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N96" s="15"/>
       <c r="O96" s="15"/>
@@ -4903,7 +4933,7 @@
       <c r="K97" s="15"/>
       <c r="L97" s="15"/>
       <c r="M97" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N97" s="15"/>
       <c r="O97" s="15"/>
@@ -4927,7 +4957,7 @@
       <c r="K98" s="15"/>
       <c r="L98" s="15"/>
       <c r="M98" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N98" s="15"/>
       <c r="O98" s="15"/>
@@ -4951,7 +4981,7 @@
       <c r="K99" s="15"/>
       <c r="L99" s="15"/>
       <c r="M99" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N99" s="15"/>
       <c r="O99" s="15"/>
@@ -4975,7 +5005,7 @@
       <c r="K100" s="15"/>
       <c r="L100" s="15"/>
       <c r="M100" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N100" s="15"/>
       <c r="O100" s="15"/>
@@ -4999,7 +5029,7 @@
       <c r="K101" s="15"/>
       <c r="L101" s="15"/>
       <c r="M101" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N101" s="15"/>
       <c r="O101" s="15"/>
@@ -5023,7 +5053,7 @@
       <c r="K102" s="15"/>
       <c r="L102" s="15"/>
       <c r="M102" s="15" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="N102" s="15"/>
       <c r="O102" s="15"/>
@@ -5035,7 +5065,7 @@
     </row>
     <row r="103" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
75ohm resistors on WM8731 MCLK and SDIO CK make both work
</commit_message>
<xml_diff>
--- a/stm32f4-discovery-pin-table.xlsx
+++ b/stm32f4-discovery-pin-table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="261">
   <si>
     <t xml:space="preserve">Main function</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t xml:space="preserve">DISCOLOTI-FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM8731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23LC1024</t>
   </si>
   <si>
     <t xml:space="preserve">BOOT0</t>
@@ -197,6 +206,9 @@
     <t xml:space="preserve">LRCK / AIN1x</t>
   </si>
   <si>
+    <t xml:space="preserve">DAC1</t>
+  </si>
+  <si>
     <t xml:space="preserve">PA5</t>
   </si>
   <si>
@@ -211,7 +223,7 @@
     <t xml:space="preserve">SCL / SPC</t>
   </si>
   <si>
-    <t xml:space="preserve">DAC (x0x pitch)?</t>
+    <t xml:space="preserve">DAC2 (x0x pitch)?</t>
   </si>
   <si>
     <t xml:space="preserve">PA6</t>
@@ -442,9 +454,6 @@
     <t xml:space="preserve">23LCV1024 SRAM?(SPI1_NSS)</t>
   </si>
   <si>
-    <t xml:space="preserve">spi3 used by audio codec.--&gt; use SPI1:PA15 NSSPA3 or PB3 SCKPA6 or PB4 MISOPA7 or PB5 MOSIALTERNATE(5)</t>
-  </si>
-  <si>
     <t xml:space="preserve">PB0</t>
   </si>
   <si>
@@ -632,6 +641,9 @@
   </si>
   <si>
     <t xml:space="preserve">SCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has 4.7k pullup</t>
   </si>
   <si>
     <t xml:space="preserve">PB7</t>
@@ -1243,6 +1255,9 @@
   <si>
     <t xml:space="preserve">FSMC_D2
 CAN1_RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN</t>
   </si>
   <si>
     <t xml:space="preserve">PD1</t>
@@ -1721,7 +1736,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1794,12 +1809,20 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1879,30 +1902,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S103"/>
+  <dimension ref="A1:V103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="V29" activeCellId="0" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="1" width="6.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="2" width="12.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="1" width="5.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="33.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="1" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="14" style="1" width="5.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="16.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="19" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="20.03"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="963" min="23" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="964" style="1" width="11.52"/>
@@ -1964,13 +1988,22 @@
       <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>94</v>
@@ -1992,10 +2025,13 @@
         <v>21</v>
       </c>
       <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="n">
@@ -2005,11 +2041,11 @@
       <c r="E3" s="7"/>
       <c r="F3" s="9"/>
       <c r="G3" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -2024,13 +2060,16 @@
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="105.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>23</v>
@@ -2039,14 +2078,14 @@
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
       <c r="G4" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
@@ -2056,15 +2095,18 @@
       </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10" t="s">
-        <v>26</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C5" s="13" t="n">
         <v>24</v>
@@ -2078,7 +2120,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -2088,15 +2130,18 @@
       </c>
       <c r="Q5" s="13"/>
       <c r="R5" s="13" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C6" s="15" t="n">
         <v>25</v>
@@ -2110,7 +2155,7 @@
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="L6" s="15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
@@ -2120,15 +2165,18 @@
       </c>
       <c r="Q6" s="15"/>
       <c r="R6" s="15" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7" s="15" t="n">
         <v>26</v>
@@ -2142,7 +2190,7 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -2152,21 +2200,24 @@
       </c>
       <c r="Q7" s="15"/>
       <c r="R7" s="15" t="s">
-        <v>35</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="105.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C8" s="7" t="n">
         <v>29</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="9"/>
@@ -2176,7 +2227,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
@@ -2185,14 +2236,19 @@
         <v>16</v>
       </c>
       <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="R8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C9" s="15" t="n">
         <v>30</v>
@@ -2200,7 +2256,7 @@
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -2208,7 +2264,7 @@
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
@@ -2218,15 +2274,18 @@
       </c>
       <c r="Q9" s="15"/>
       <c r="R9" s="15" t="s">
-        <v>42</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C10" s="15" t="n">
         <v>31</v>
@@ -2234,7 +2293,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="16" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
@@ -2242,7 +2301,7 @@
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
@@ -2252,15 +2311,18 @@
       </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="15" t="s">
-        <v>46</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C11" s="15" t="n">
         <v>32</v>
@@ -2268,7 +2330,7 @@
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="16" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -2276,7 +2338,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
@@ -2286,15 +2348,18 @@
       </c>
       <c r="Q11" s="15"/>
       <c r="R11" s="15" t="s">
-        <v>50</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C12" s="15" t="n">
         <v>67</v>
@@ -2308,7 +2373,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
       <c r="L12" s="15" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -2318,13 +2383,16 @@
         <v>43</v>
       </c>
       <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C13" s="7" t="n">
         <v>68</v>
@@ -2334,15 +2402,15 @@
       <c r="F13" s="9"/>
       <c r="G13" s="7"/>
       <c r="H13" s="8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M13" s="7"/>
       <c r="N13" s="7" t="n">
@@ -2354,13 +2422,16 @@
         <v>44</v>
       </c>
       <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C14" s="7" t="n">
         <v>69</v>
@@ -2372,11 +2443,11 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7" t="n">
@@ -2388,13 +2459,16 @@
         <v>41</v>
       </c>
       <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C15" s="7" t="n">
         <v>70</v>
@@ -2406,11 +2480,11 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="M15" s="7"/>
       <c r="N15" s="7" t="n">
@@ -2420,13 +2494,16 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C16" s="7" t="n">
         <v>71</v>
@@ -2438,11 +2515,11 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7" t="n">
@@ -2452,13 +2529,16 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C17" s="7" t="n">
         <v>72</v>
@@ -2469,12 +2549,12 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="8" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
@@ -2486,13 +2566,16 @@
         <v>42</v>
       </c>
       <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C18" s="7" t="n">
         <v>76</v>
@@ -2503,12 +2586,12 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
@@ -2520,13 +2603,16 @@
         <v>39</v>
       </c>
       <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C19" s="10" t="n">
         <v>77</v>
@@ -2540,7 +2626,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
@@ -2549,19 +2635,19 @@
       <c r="Q19" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="R19" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>75</v>
+      <c r="R19" s="18"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>35</v>
@@ -2575,7 +2661,7 @@
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
       <c r="L20" s="15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
@@ -2585,15 +2671,18 @@
       </c>
       <c r="Q20" s="15"/>
       <c r="R20" s="15" t="s">
-        <v>78</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C21" s="15" t="n">
         <v>36</v>
@@ -2607,7 +2696,7 @@
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
       <c r="L21" s="15" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
@@ -2617,15 +2706,18 @@
       </c>
       <c r="Q21" s="15"/>
       <c r="R21" s="15" t="s">
-        <v>81</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C22" s="7" t="n">
         <v>37</v>
@@ -2639,7 +2731,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
@@ -2649,13 +2741,16 @@
       </c>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C23" s="10" t="n">
         <v>89</v>
@@ -2666,12 +2761,12 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
@@ -2682,16 +2777,19 @@
       <c r="Q23" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="R23" s="10" t="s">
-        <v>88</v>
+      <c r="R23" s="18"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C24" s="10" t="n">
         <v>90</v>
@@ -2705,7 +2803,7 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
@@ -2714,16 +2812,19 @@
       <c r="Q24" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="R24" s="10" t="s">
-        <v>91</v>
+      <c r="R24" s="18"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="118.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="s">
-        <v>92</v>
+      <c r="A25" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C25" s="10" t="n">
         <v>91</v>
@@ -2737,7 +2838,7 @@
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
@@ -2746,22 +2847,25 @@
       <c r="Q25" s="10" t="n">
         <v>26</v>
       </c>
-      <c r="R25" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R25" s="18"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C26" s="7" t="n">
         <v>92</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="9"/>
@@ -2771,7 +2875,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -2781,13 +2885,19 @@
         <v>23</v>
       </c>
       <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>93</v>
@@ -2801,7 +2911,7 @@
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
@@ -2811,13 +2921,16 @@
         <v>24</v>
       </c>
       <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="105.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C28" s="15" t="n">
         <v>95</v>
@@ -2831,7 +2944,7 @@
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="15" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
@@ -2841,19 +2954,22 @@
         <v>19</v>
       </c>
       <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="118.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C29" s="7" t="n">
         <v>96</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="9"/>
@@ -2863,7 +2979,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
@@ -2873,20 +2989,26 @@
         <v>20</v>
       </c>
       <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="105.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C30" s="10" t="n">
         <v>47</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="10"/>
@@ -2895,7 +3017,7 @@
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
       <c r="L30" s="10" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
@@ -2904,17 +3026,19 @@
         <v>34</v>
       </c>
       <c r="Q30" s="10"/>
-      <c r="R30" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="S30" s="3"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>114</v>
       </c>
       <c r="C31" s="10" t="n">
         <v>48</v>
@@ -2928,7 +3052,7 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
@@ -2937,17 +3061,19 @@
         <v>35</v>
       </c>
       <c r="Q31" s="10"/>
-      <c r="R31" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="S31" s="3"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="131.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C32" s="10" t="n">
         <v>51</v>
@@ -2961,7 +3087,7 @@
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="10" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
@@ -2970,17 +3096,19 @@
         <v>36</v>
       </c>
       <c r="Q32" s="10"/>
-      <c r="R32" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="S32" s="3"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="118.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C33" s="10" t="n">
         <v>52</v>
@@ -2994,7 +3122,7 @@
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
       <c r="L33" s="10" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
@@ -3003,17 +3131,19 @@
         <v>37</v>
       </c>
       <c r="Q33" s="10"/>
-      <c r="R33" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="S33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="92.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R33" s="18"/>
+      <c r="S33" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+    </row>
+    <row r="34" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C34" s="10" t="n">
         <v>53</v>
@@ -3027,7 +3157,7 @@
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
       <c r="L34" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
@@ -3036,17 +3166,19 @@
         <v>38</v>
       </c>
       <c r="Q34" s="10"/>
-      <c r="R34" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="S34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R34" s="18"/>
+      <c r="S34" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+    </row>
+    <row r="35" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C35" s="10" t="n">
         <v>54</v>
@@ -3060,7 +3192,7 @@
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
@@ -3069,17 +3201,19 @@
         <v>39</v>
       </c>
       <c r="Q35" s="10"/>
-      <c r="R35" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="S35" s="3"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C36" s="7" t="n">
         <v>15</v>
@@ -3091,11 +3225,11 @@
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="17" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="K36" s="7"/>
       <c r="L36" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
@@ -3105,14 +3239,16 @@
       </c>
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
-      <c r="S36" s="3"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C37" s="15" t="n">
         <v>16</v>
@@ -3126,7 +3262,7 @@
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
       <c r="L37" s="15" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
@@ -3136,16 +3272,18 @@
       </c>
       <c r="Q37" s="15"/>
       <c r="R37" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="S37" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="S37" s="21"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
     </row>
     <row r="38" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C38" s="15" t="n">
         <v>17</v>
@@ -3159,7 +3297,7 @@
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
@@ -3169,21 +3307,23 @@
       </c>
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
-      <c r="S38" s="3"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
     </row>
     <row r="39" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C39" s="15" t="n">
         <v>18</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="15" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F39" s="16"/>
       <c r="G39" s="15"/>
@@ -3192,7 +3332,7 @@
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
@@ -3202,14 +3342,16 @@
       </c>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
-      <c r="S39" s="3"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="15"/>
     </row>
     <row r="40" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="15" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C40" s="15" t="n">
         <v>33</v>
@@ -3223,7 +3365,7 @@
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
       <c r="L40" s="15" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
@@ -3233,14 +3375,16 @@
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
-      <c r="S40" s="3"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
     </row>
     <row r="41" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="15" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C41" s="15" t="n">
         <v>34</v>
@@ -3254,7 +3398,7 @@
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
       <c r="L41" s="15" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
@@ -3264,14 +3408,16 @@
       </c>
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
-      <c r="S41" s="3"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="15"/>
     </row>
     <row r="42" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>140</v>
+        <v>143</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>144</v>
       </c>
       <c r="C42" s="10" t="n">
         <v>63</v>
@@ -3285,7 +3431,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
       <c r="L42" s="10" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
@@ -3294,23 +3440,25 @@
       <c r="Q42" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="R42" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="S42" s="3"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C43" s="7" t="n">
         <v>64</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="9"/>
@@ -3320,7 +3468,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
       <c r="L43" s="7" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
@@ -3330,83 +3478,92 @@
         <v>48</v>
       </c>
       <c r="R43" s="7"/>
-    </row>
-    <row r="44" customFormat="false" ht="66.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="15" t="n">
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="66.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="10" t="n">
         <v>65</v>
       </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15" t="n">
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="R44" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="92.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="15" t="n">
+      <c r="R44" s="18"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="U44" s="10"/>
+    </row>
+    <row r="45" customFormat="false" ht="92.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="10" t="n">
         <v>66</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15" t="n">
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="R45" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R45" s="18"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="U45" s="10"/>
+    </row>
+    <row r="46" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C46" s="7" t="n">
         <v>78</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="9"/>
@@ -3416,7 +3573,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
@@ -3425,54 +3582,60 @@
       <c r="Q46" s="7" t="n">
         <v>37</v>
       </c>
-      <c r="R46" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="15" t="n">
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="U46" s="10"/>
+    </row>
+    <row r="47" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="10" t="n">
         <v>79</v>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15" t="n">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="R47" s="10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="79.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R47" s="18"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="U47" s="10"/>
+    </row>
+    <row r="48" customFormat="false" ht="79.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C48" s="7" t="n">
         <v>80</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="9"/>
@@ -3482,7 +3645,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -3491,16 +3654,19 @@
       <c r="Q48" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="R48" s="10" t="s">
-        <v>161</v>
-      </c>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="U48" s="10"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="15" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C49" s="15" t="n">
         <v>7</v>
@@ -3514,7 +3680,7 @@
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
       <c r="L49" s="15" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
@@ -3524,13 +3690,16 @@
         <v>12</v>
       </c>
       <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="15" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C50" s="15" t="n">
         <v>8</v>
@@ -3543,10 +3712,10 @@
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="L50" s="15" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
@@ -3556,13 +3725,16 @@
         <v>9</v>
       </c>
       <c r="R50" s="15"/>
+      <c r="S50" s="15"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="15" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C51" s="15" t="n">
         <v>9</v>
@@ -3575,10 +3747,10 @@
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="L51" s="15" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
@@ -3588,13 +3760,16 @@
         <v>10</v>
       </c>
       <c r="R51" s="15"/>
-    </row>
-    <row r="52" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S51" s="15"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="15"/>
+    </row>
+    <row r="52" customFormat="false" ht="27.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C52" s="15" t="n">
         <v>81</v>
@@ -3608,7 +3783,7 @@
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
       <c r="L52" s="15" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
@@ -3618,13 +3793,19 @@
         <v>36</v>
       </c>
       <c r="R52" s="15"/>
-    </row>
-    <row r="53" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S52" s="15"/>
+      <c r="T52" s="15"/>
+      <c r="U52" s="15"/>
+      <c r="V52" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="27.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="15" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C53" s="15" t="n">
         <v>82</v>
@@ -3638,7 +3819,7 @@
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
       <c r="L53" s="15" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -3648,13 +3829,19 @@
         <v>33</v>
       </c>
       <c r="R53" s="15"/>
-    </row>
-    <row r="54" customFormat="false" ht="53.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S53" s="15"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="15"/>
+      <c r="V53" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C54" s="10" t="n">
         <v>83</v>
@@ -3668,7 +3855,7 @@
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
       <c r="L54" s="10" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
@@ -3677,16 +3864,19 @@
       <c r="Q54" s="10" t="n">
         <v>34</v>
       </c>
-      <c r="R54" s="10" t="s">
-        <v>176</v>
-      </c>
+      <c r="R54" s="18"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="U54" s="10"/>
     </row>
     <row r="55" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C55" s="15" t="n">
         <v>84</v>
@@ -3700,7 +3890,7 @@
       <c r="J55" s="15"/>
       <c r="K55" s="15"/>
       <c r="L55" s="15" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
@@ -3710,19 +3900,22 @@
         <v>31</v>
       </c>
       <c r="R55" s="15"/>
+      <c r="S55" s="15"/>
+      <c r="T55" s="15"/>
+      <c r="U55" s="15"/>
     </row>
     <row r="56" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C56" s="7" t="n">
         <v>85</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="9"/>
@@ -3732,7 +3925,7 @@
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
@@ -3742,13 +3935,16 @@
         <v>32</v>
       </c>
       <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C57" s="7" t="n">
         <v>86</v>
@@ -3758,15 +3954,15 @@
       <c r="F57" s="9"/>
       <c r="G57" s="7"/>
       <c r="H57" s="8" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I57" s="7"/>
       <c r="J57" s="8" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="K57" s="7"/>
       <c r="L57" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
@@ -3776,13 +3972,16 @@
         <v>29</v>
       </c>
       <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C58" s="15" t="n">
         <v>87</v>
@@ -3796,7 +3995,7 @@
       <c r="J58" s="15"/>
       <c r="K58" s="15"/>
       <c r="L58" s="15" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
@@ -3806,13 +4005,16 @@
         <v>30</v>
       </c>
       <c r="R58" s="15"/>
+      <c r="S58" s="15"/>
+      <c r="T58" s="15"/>
+      <c r="U58" s="15"/>
     </row>
     <row r="59" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="15" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C59" s="15" t="n">
         <v>88</v>
@@ -3826,7 +4028,7 @@
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
@@ -3836,13 +4038,16 @@
         <v>27</v>
       </c>
       <c r="R59" s="15"/>
+      <c r="S59" s="15"/>
+      <c r="T59" s="15"/>
+      <c r="U59" s="15"/>
     </row>
     <row r="60" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C60" s="10" t="n">
         <v>55</v>
@@ -3856,7 +4061,7 @@
       <c r="J60" s="10"/>
       <c r="K60" s="10"/>
       <c r="L60" s="10" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="M60" s="10"/>
       <c r="N60" s="10"/>
@@ -3866,15 +4071,18 @@
       </c>
       <c r="Q60" s="10"/>
       <c r="R60" s="10" t="s">
-        <v>191</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="S60" s="10"/>
+      <c r="T60" s="10"/>
+      <c r="U60" s="10"/>
     </row>
     <row r="61" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C61" s="10" t="n">
         <v>56</v>
@@ -3888,7 +4096,7 @@
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
       <c r="L61" s="10" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="M61" s="10"/>
       <c r="N61" s="10"/>
@@ -3898,15 +4106,18 @@
       </c>
       <c r="Q61" s="10"/>
       <c r="R61" s="10" t="s">
-        <v>194</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="S61" s="10"/>
+      <c r="T61" s="10"/>
+      <c r="U61" s="10"/>
     </row>
     <row r="62" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C62" s="15" t="n">
         <v>57</v>
@@ -3920,7 +4131,7 @@
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
       <c r="L62" s="15" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
@@ -3930,13 +4141,16 @@
       </c>
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
+      <c r="S62" s="15"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="15"/>
     </row>
     <row r="63" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C63" s="15" t="n">
         <v>58</v>
@@ -3950,7 +4164,7 @@
       <c r="J63" s="15"/>
       <c r="K63" s="15"/>
       <c r="L63" s="15" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
@@ -3960,13 +4174,16 @@
       </c>
       <c r="Q63" s="15"/>
       <c r="R63" s="15"/>
+      <c r="S63" s="15"/>
+      <c r="T63" s="15"/>
+      <c r="U63" s="15"/>
     </row>
     <row r="64" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C64" s="10" t="n">
         <v>59</v>
@@ -3976,13 +4193,13 @@
       <c r="F64" s="11"/>
       <c r="G64" s="10"/>
       <c r="H64" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I64" s="10"/>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
       <c r="L64" s="10" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
@@ -3994,13 +4211,16 @@
       <c r="R64" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="S64" s="10"/>
+      <c r="T64" s="10"/>
+      <c r="U64" s="10"/>
     </row>
     <row r="65" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C65" s="10" t="n">
         <v>60</v>
@@ -4010,13 +4230,13 @@
       <c r="F65" s="11"/>
       <c r="G65" s="10"/>
       <c r="H65" s="12" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="I65" s="10"/>
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
       <c r="L65" s="10" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
@@ -4028,13 +4248,16 @@
       <c r="R65" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="10"/>
     </row>
     <row r="66" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C66" s="10" t="n">
         <v>61</v>
@@ -4044,13 +4267,13 @@
       <c r="F66" s="11"/>
       <c r="G66" s="10"/>
       <c r="H66" s="12" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I66" s="10"/>
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
       <c r="L66" s="10" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
@@ -4062,13 +4285,16 @@
       <c r="R66" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="10"/>
     </row>
     <row r="67" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C67" s="10" t="n">
         <v>62</v>
@@ -4078,13 +4304,13 @@
       <c r="F67" s="11"/>
       <c r="G67" s="10"/>
       <c r="H67" s="12" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="I67" s="10"/>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
       <c r="L67" s="10" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
@@ -4096,13 +4322,16 @@
       <c r="R67" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
+      <c r="U67" s="10"/>
     </row>
     <row r="68" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C68" s="15" t="n">
         <v>97</v>
@@ -4110,7 +4339,7 @@
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
       <c r="F68" s="16" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="15"/>
@@ -4118,7 +4347,7 @@
       <c r="J68" s="15"/>
       <c r="K68" s="15"/>
       <c r="L68" s="15" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
@@ -4128,13 +4357,16 @@
         <v>17</v>
       </c>
       <c r="R68" s="15"/>
+      <c r="S68" s="15"/>
+      <c r="T68" s="15"/>
+      <c r="U68" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C69" s="15" t="n">
         <v>98</v>
@@ -4142,7 +4374,7 @@
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
       <c r="F69" s="16" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="15"/>
@@ -4150,7 +4382,7 @@
       <c r="J69" s="15"/>
       <c r="K69" s="15"/>
       <c r="L69" s="15" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
@@ -4160,13 +4392,16 @@
         <v>18</v>
       </c>
       <c r="R69" s="15"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+      <c r="U69" s="15"/>
     </row>
     <row r="70" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="15" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C70" s="15" t="n">
         <v>1</v>
@@ -4180,7 +4415,7 @@
       <c r="J70" s="15"/>
       <c r="K70" s="15"/>
       <c r="L70" s="15" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
@@ -4190,13 +4425,16 @@
         <v>15</v>
       </c>
       <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C71" s="15" t="n">
         <v>2</v>
@@ -4204,7 +4442,7 @@
       <c r="D71" s="15"/>
       <c r="E71" s="15"/>
       <c r="F71" s="16" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="15"/>
@@ -4212,7 +4450,7 @@
       <c r="J71" s="15"/>
       <c r="K71" s="15"/>
       <c r="L71" s="15" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
@@ -4222,13 +4460,16 @@
         <v>16</v>
       </c>
       <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="15" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C72" s="15" t="n">
         <v>3</v>
@@ -4242,7 +4483,7 @@
       <c r="J72" s="15"/>
       <c r="K72" s="15"/>
       <c r="L72" s="15" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
@@ -4252,13 +4493,16 @@
         <v>13</v>
       </c>
       <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C73" s="15" t="n">
         <v>4</v>
@@ -4272,7 +4516,7 @@
       <c r="J73" s="15"/>
       <c r="K73" s="15"/>
       <c r="L73" s="15" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
@@ -4282,13 +4526,16 @@
         <v>14</v>
       </c>
       <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
     </row>
     <row r="74" customFormat="false" ht="53.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="15" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C74" s="15" t="n">
         <v>5</v>
@@ -4302,7 +4549,7 @@
       <c r="J74" s="15"/>
       <c r="K74" s="15"/>
       <c r="L74" s="15" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="M74" s="15"/>
       <c r="N74" s="15"/>
@@ -4312,13 +4559,16 @@
         <v>11</v>
       </c>
       <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
     </row>
     <row r="75" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="15" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C75" s="15" t="n">
         <v>38</v>
@@ -4332,7 +4582,7 @@
       <c r="J75" s="15"/>
       <c r="K75" s="15"/>
       <c r="L75" s="15" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
@@ -4342,13 +4592,16 @@
       </c>
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="15" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C76" s="15" t="n">
         <v>39</v>
@@ -4362,7 +4615,7 @@
       <c r="J76" s="15"/>
       <c r="K76" s="15"/>
       <c r="L76" s="15" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
@@ -4372,13 +4625,16 @@
       </c>
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="15" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C77" s="15" t="n">
         <v>40</v>
@@ -4392,7 +4648,7 @@
       <c r="J77" s="15"/>
       <c r="K77" s="15"/>
       <c r="L77" s="15" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
@@ -4402,13 +4658,16 @@
       </c>
       <c r="Q77" s="15"/>
       <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
     </row>
     <row r="78" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="15" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C78" s="15" t="n">
         <v>41</v>
@@ -4422,7 +4681,7 @@
       <c r="J78" s="15"/>
       <c r="K78" s="15"/>
       <c r="L78" s="15" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
@@ -4432,13 +4691,16 @@
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="15" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C79" s="15" t="n">
         <v>42</v>
@@ -4452,7 +4714,7 @@
       <c r="J79" s="15"/>
       <c r="K79" s="15"/>
       <c r="L79" s="15" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
@@ -4462,13 +4724,16 @@
       </c>
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
+      <c r="S79" s="15"/>
+      <c r="T79" s="15"/>
+      <c r="U79" s="15"/>
     </row>
     <row r="80" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="15" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C80" s="15" t="n">
         <v>43</v>
@@ -4482,7 +4747,7 @@
       <c r="J80" s="15"/>
       <c r="K80" s="15"/>
       <c r="L80" s="15" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="M80" s="15"/>
       <c r="N80" s="15"/>
@@ -4492,13 +4757,16 @@
       </c>
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
+      <c r="S80" s="15"/>
+      <c r="T80" s="15"/>
+      <c r="U80" s="15"/>
     </row>
     <row r="81" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="15" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C81" s="15" t="n">
         <v>44</v>
@@ -4512,7 +4780,7 @@
       <c r="J81" s="15"/>
       <c r="K81" s="15"/>
       <c r="L81" s="15" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="M81" s="15"/>
       <c r="N81" s="15"/>
@@ -4522,13 +4790,16 @@
       </c>
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
+      <c r="S81" s="15"/>
+      <c r="T81" s="15"/>
+      <c r="U81" s="15"/>
     </row>
     <row r="82" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="15" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C82" s="15" t="n">
         <v>45</v>
@@ -4542,7 +4813,7 @@
       <c r="J82" s="15"/>
       <c r="K82" s="15"/>
       <c r="L82" s="15" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="M82" s="15"/>
       <c r="N82" s="15"/>
@@ -4552,13 +4823,16 @@
       </c>
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
+      <c r="S82" s="15"/>
+      <c r="T82" s="15"/>
+      <c r="U82" s="15"/>
     </row>
     <row r="83" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C83" s="15" t="n">
         <v>46</v>
@@ -4572,7 +4846,7 @@
       <c r="J83" s="15"/>
       <c r="K83" s="15"/>
       <c r="L83" s="15" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="M83" s="15"/>
       <c r="N83" s="15"/>
@@ -4582,13 +4856,16 @@
       </c>
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
+      <c r="S83" s="15"/>
+      <c r="T83" s="15"/>
+      <c r="U83" s="15"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C84" s="7" t="n">
         <v>12</v>
@@ -4601,10 +4878,10 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="17" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="L84" s="7" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
@@ -4614,13 +4891,16 @@
         <v>7</v>
       </c>
       <c r="R84" s="7"/>
+      <c r="S84" s="7"/>
+      <c r="T84" s="7"/>
+      <c r="U84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C85" s="7" t="n">
         <v>13</v>
@@ -4633,10 +4913,10 @@
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
       <c r="K85" s="17" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="L85" s="7" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
@@ -4646,6 +4926,9 @@
         <v>8</v>
       </c>
       <c r="R85" s="7"/>
+      <c r="S85" s="7"/>
+      <c r="T85" s="7"/>
+      <c r="U85" s="7"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="15"/>
@@ -4661,7 +4944,7 @@
       <c r="K86" s="15"/>
       <c r="L86" s="15"/>
       <c r="M86" s="15" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="N86" s="15"/>
       <c r="O86" s="15"/>
@@ -4670,6 +4953,9 @@
         <v>3</v>
       </c>
       <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15"/>
+      <c r="U86" s="15"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="15"/>
@@ -4685,7 +4971,7 @@
       <c r="K87" s="15"/>
       <c r="L87" s="15"/>
       <c r="M87" s="15" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="N87" s="15"/>
       <c r="O87" s="15"/>
@@ -4694,6 +4980,9 @@
         <v>4</v>
       </c>
       <c r="R87" s="15"/>
+      <c r="S87" s="15"/>
+      <c r="T87" s="15"/>
+      <c r="U87" s="15"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="15"/>
@@ -4709,7 +4998,7 @@
       <c r="K88" s="15"/>
       <c r="L88" s="15"/>
       <c r="M88" s="15" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="N88" s="15"/>
       <c r="O88" s="15"/>
@@ -4718,6 +5007,9 @@
         <v>5</v>
       </c>
       <c r="R88" s="15"/>
+      <c r="S88" s="15"/>
+      <c r="T88" s="15"/>
+      <c r="U88" s="15"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="15"/>
@@ -4733,7 +5025,7 @@
       <c r="K89" s="15"/>
       <c r="L89" s="15"/>
       <c r="M89" s="15" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="N89" s="15"/>
       <c r="O89" s="15"/>
@@ -4742,6 +5034,9 @@
         <v>6</v>
       </c>
       <c r="R89" s="15"/>
+      <c r="S89" s="15"/>
+      <c r="T89" s="15"/>
+      <c r="U89" s="15"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="15"/>
@@ -4757,7 +5052,7 @@
       <c r="K90" s="15"/>
       <c r="L90" s="15"/>
       <c r="M90" s="15" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="N90" s="15"/>
       <c r="O90" s="15"/>
@@ -4766,6 +5061,9 @@
       </c>
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
+      <c r="S90" s="15"/>
+      <c r="T90" s="15"/>
+      <c r="U90" s="15"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="15"/>
@@ -4781,7 +5079,7 @@
       <c r="K91" s="15"/>
       <c r="L91" s="15"/>
       <c r="M91" s="15" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="N91" s="15"/>
       <c r="O91" s="15"/>
@@ -4790,6 +5088,9 @@
       </c>
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
+      <c r="S91" s="15"/>
+      <c r="T91" s="15"/>
+      <c r="U91" s="15"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="15"/>
@@ -4805,7 +5106,7 @@
       <c r="K92" s="15"/>
       <c r="L92" s="15"/>
       <c r="M92" s="15" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="N92" s="15"/>
       <c r="O92" s="15"/>
@@ -4814,6 +5115,9 @@
         <v>22</v>
       </c>
       <c r="R92" s="15"/>
+      <c r="S92" s="15"/>
+      <c r="T92" s="15"/>
+      <c r="U92" s="15"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="15"/>
@@ -4825,15 +5129,15 @@
       <c r="G93" s="15"/>
       <c r="H93" s="15"/>
       <c r="I93" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="J93" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="K93" s="15"/>
       <c r="L93" s="15"/>
       <c r="M93" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N93" s="15" t="n">
         <v>5</v>
@@ -4846,6 +5150,9 @@
       </c>
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
+      <c r="S93" s="15"/>
+      <c r="T93" s="15"/>
+      <c r="U93" s="15"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="15"/>
@@ -4861,7 +5168,7 @@
       <c r="K94" s="15"/>
       <c r="L94" s="15"/>
       <c r="M94" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N94" s="15"/>
       <c r="O94" s="15"/>
@@ -4870,6 +5177,9 @@
       </c>
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
+      <c r="S94" s="15"/>
+      <c r="T94" s="15"/>
+      <c r="U94" s="15"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="15"/>
@@ -4885,7 +5195,7 @@
       <c r="K95" s="15"/>
       <c r="L95" s="15"/>
       <c r="M95" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N95" s="15"/>
       <c r="O95" s="15"/>
@@ -4894,6 +5204,9 @@
       </c>
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
+      <c r="S95" s="15"/>
+      <c r="T95" s="15"/>
+      <c r="U95" s="15"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="15"/>
@@ -4909,7 +5222,7 @@
       <c r="K96" s="15"/>
       <c r="L96" s="15"/>
       <c r="M96" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N96" s="15"/>
       <c r="O96" s="15"/>
@@ -4918,6 +5231,9 @@
       </c>
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
+      <c r="S96" s="15"/>
+      <c r="T96" s="15"/>
+      <c r="U96" s="15"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="15"/>
@@ -4933,7 +5249,7 @@
       <c r="K97" s="15"/>
       <c r="L97" s="15"/>
       <c r="M97" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N97" s="15"/>
       <c r="O97" s="15"/>
@@ -4942,6 +5258,9 @@
       </c>
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
+      <c r="S97" s="15"/>
+      <c r="T97" s="15"/>
+      <c r="U97" s="15"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="15"/>
@@ -4957,7 +5276,7 @@
       <c r="K98" s="15"/>
       <c r="L98" s="15"/>
       <c r="M98" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N98" s="15"/>
       <c r="O98" s="15"/>
@@ -4966,6 +5285,9 @@
       </c>
       <c r="Q98" s="15"/>
       <c r="R98" s="15"/>
+      <c r="S98" s="15"/>
+      <c r="T98" s="15"/>
+      <c r="U98" s="15"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="15"/>
@@ -4981,7 +5303,7 @@
       <c r="K99" s="15"/>
       <c r="L99" s="15"/>
       <c r="M99" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N99" s="15"/>
       <c r="O99" s="15"/>
@@ -4990,6 +5312,9 @@
         <v>1</v>
       </c>
       <c r="R99" s="15"/>
+      <c r="S99" s="15"/>
+      <c r="T99" s="15"/>
+      <c r="U99" s="15"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="15"/>
@@ -5005,7 +5330,7 @@
       <c r="K100" s="15"/>
       <c r="L100" s="15"/>
       <c r="M100" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N100" s="15"/>
       <c r="O100" s="15"/>
@@ -5014,6 +5339,9 @@
         <v>2</v>
       </c>
       <c r="R100" s="15"/>
+      <c r="S100" s="15"/>
+      <c r="T100" s="15"/>
+      <c r="U100" s="15"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="15"/>
@@ -5029,7 +5357,7 @@
       <c r="K101" s="15"/>
       <c r="L101" s="15"/>
       <c r="M101" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N101" s="15"/>
       <c r="O101" s="15"/>
@@ -5038,6 +5366,9 @@
         <v>49</v>
       </c>
       <c r="R101" s="15"/>
+      <c r="S101" s="15"/>
+      <c r="T101" s="15"/>
+      <c r="U101" s="15"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="15"/>
@@ -5053,7 +5384,7 @@
       <c r="K102" s="15"/>
       <c r="L102" s="15"/>
       <c r="M102" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="N102" s="15"/>
       <c r="O102" s="15"/>
@@ -5062,10 +5393,13 @@
         <v>50</v>
       </c>
       <c r="R102" s="15"/>
+      <c r="S102" s="15"/>
+      <c r="T102" s="15"/>
+      <c r="U102" s="15"/>
     </row>
     <row r="103" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="1" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kicad pcb backup, hohum axoctrl study
</commit_message>
<xml_diff>
--- a/stm32f4-discovery-pin-table.xlsx
+++ b/stm32f4-discovery-pin-table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="267">
   <si>
     <t xml:space="preserve">Main function</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t xml:space="preserve">AIN6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPI3_NSS2</t>
   </si>
   <si>
     <t xml:space="preserve">PB1</t>
@@ -664,6 +667,9 @@
     <t xml:space="preserve">SCL</t>
   </si>
   <si>
+    <t xml:space="preserve">I2C1_HEADER</t>
+  </si>
+  <si>
     <t xml:space="preserve">Has 4.7k pullup</t>
   </si>
   <si>
@@ -780,9 +786,6 @@
     <t xml:space="preserve">WM8731_SCL</t>
   </si>
   <si>
-    <t xml:space="preserve">OLED_SCL</t>
-  </si>
-  <si>
     <t xml:space="preserve">PB11</t>
   </si>
   <si>
@@ -814,9 +817,6 @@
   </si>
   <si>
     <t xml:space="preserve">WM8731_SDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OLED_SDA</t>
   </si>
   <si>
     <t xml:space="preserve">PB12</t>
@@ -1580,7 +1580,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1643,6 +1643,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00A65D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1718,7 +1724,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1789,6 +1795,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1883,9 +1893,9 @@
   <dimension ref="A1:W103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="V11" activeCellId="0" sqref="V11"/>
+      <selection pane="bottomLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2647,47 +2657,50 @@
       <c r="V19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="80.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="14" t="n">
+      <c r="C20" s="9" t="n">
         <v>35</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14" t="s">
+      <c r="D20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14" t="n">
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14" t="s">
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="18" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="93.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C21" s="14" t="n">
         <v>36</v>
@@ -2701,7 +2714,7 @@
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
@@ -2711,7 +2724,7 @@
       </c>
       <c r="Q21" s="14"/>
       <c r="R21" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
@@ -2720,10 +2733,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>37</v>
@@ -2737,7 +2750,7 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -2754,10 +2767,10 @@
     </row>
     <row r="23" customFormat="false" ht="80.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C23" s="9" t="n">
         <v>89</v>
@@ -2767,13 +2780,13 @@
       <c r="F23" s="10"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="18" t="s">
-        <v>93</v>
+      <c r="I23" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -2788,16 +2801,16 @@
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
       <c r="U23" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="V23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C24" s="9" t="n">
         <v>90</v>
@@ -2811,7 +2824,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
@@ -2824,16 +2837,16 @@
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
       <c r="U24" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="V24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="120.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="s">
-        <v>99</v>
+      <c r="A25" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C25" s="9" t="n">
         <v>91</v>
@@ -2847,7 +2860,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -2860,55 +2873,57 @@
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
       <c r="U25" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="V25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="80.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="16" t="s">
+      <c r="A26" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="6" t="n">
+      <c r="B26" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="9" t="n">
         <v>92</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6" t="n">
+      <c r="D26" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
+      <c r="R26" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
       <c r="W26" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C27" s="14" t="n">
         <v>93</v>
@@ -2922,7 +2937,7 @@
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
       <c r="L27" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
@@ -2939,10 +2954,10 @@
     </row>
     <row r="28" customFormat="false" ht="107.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C28" s="14" t="n">
         <v>95</v>
@@ -2956,7 +2971,7 @@
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M28" s="14"/>
       <c r="N28" s="14"/>
@@ -2971,58 +2986,60 @@
       <c r="U28" s="14"/>
       <c r="V28" s="14"/>
     </row>
-    <row r="29" customFormat="false" ht="120.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="6" t="n">
+    <row r="29" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="9" t="n">
         <v>96</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6" t="n">
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
+      <c r="R29" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
       <c r="W29" s="14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="107.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C30" s="9" t="n">
         <v>47</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="9"/>
@@ -3031,7 +3048,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
@@ -3042,21 +3059,19 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="T30" s="9"/>
       <c r="U30" s="9"/>
       <c r="V30" s="9"/>
-      <c r="W30" s="14" t="s">
-        <v>117</v>
-      </c>
+      <c r="W30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="93.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="18" t="s">
         <v>119</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="C31" s="9" t="n">
         <v>48</v>
@@ -3070,7 +3085,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
@@ -3081,14 +3096,12 @@
       <c r="Q31" s="9"/>
       <c r="R31" s="17"/>
       <c r="S31" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>
       <c r="V31" s="9"/>
-      <c r="W31" s="14" t="s">
-        <v>121</v>
-      </c>
+      <c r="W31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="133.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
@@ -3301,7 +3314,7 @@
       <c r="R37" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="S37" s="20"/>
+      <c r="S37" s="21"/>
       <c r="T37" s="14"/>
       <c r="U37" s="14"/>
       <c r="V37" s="14"/>
@@ -3335,7 +3348,7 @@
       </c>
       <c r="Q38" s="14"/>
       <c r="R38" s="14"/>
-      <c r="S38" s="20"/>
+      <c r="S38" s="21"/>
       <c r="T38" s="14"/>
       <c r="U38" s="14"/>
       <c r="V38" s="14"/>
@@ -3371,7 +3384,7 @@
       </c>
       <c r="Q39" s="14"/>
       <c r="R39" s="14"/>
-      <c r="S39" s="20"/>
+      <c r="S39" s="21"/>
       <c r="T39" s="14"/>
       <c r="U39" s="14"/>
       <c r="V39" s="14"/>
@@ -3405,7 +3418,7 @@
       </c>
       <c r="Q40" s="14"/>
       <c r="R40" s="14"/>
-      <c r="S40" s="20"/>
+      <c r="S40" s="21"/>
       <c r="T40" s="14"/>
       <c r="U40" s="14"/>
       <c r="V40" s="14"/>
@@ -3439,7 +3452,7 @@
       </c>
       <c r="Q41" s="14"/>
       <c r="R41" s="14"/>
-      <c r="S41" s="20"/>
+      <c r="S41" s="21"/>
       <c r="T41" s="14"/>
       <c r="U41" s="14"/>
       <c r="V41" s="14"/>
@@ -3448,7 +3461,7 @@
       <c r="A42" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="19" t="s">
         <v>150</v>
       </c>
       <c r="C42" s="9" t="n">

</xml_diff>